<commit_message>
update script for power play variables
</commit_message>
<xml_diff>
--- a/Scraping Scripts and Template/Template.xlsx
+++ b/Scraping Scripts and Template/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="49">
   <si>
     <t>Year</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>Team2</t>
+  </si>
+  <si>
+    <t>Washington Capitals/Carolina Hurricanes</t>
+  </si>
+  <si>
+    <t>San Jose Sharks/Vegas Golden Knights</t>
+  </si>
+  <si>
+    <t>New York Islanders/Washington Capitals</t>
   </si>
 </sst>
 </file>
@@ -576,17 +585,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="E205" sqref="E205"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4985,6 +4995,86 @@
         <v>23</v>
       </c>
     </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F205" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F206" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C207" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E207" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F207" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F208" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add new variable. prepare for next round
</commit_message>
<xml_diff>
--- a/Scraping Scripts and Template/Template.xlsx
+++ b/Scraping Scripts and Template/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="48">
   <si>
     <t>Year</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Washington Capitals/Carolina Hurricanes</t>
-  </si>
-  <si>
-    <t>San Jose Sharks/Vegas Golden Knights</t>
   </si>
   <si>
     <t>New York Islanders/Washington Capitals</t>
@@ -587,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="E207" sqref="E207"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5029,7 +5026,7 @@
         <v>20</v>
       </c>
       <c r="E206" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F206" s="5" t="s">
         <v>24</v>
@@ -5060,7 +5057,7 @@
         <v>2019</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>9</v>
@@ -5069,7 +5066,7 @@
         <v>21</v>
       </c>
       <c r="E208" s="5" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F208" s="5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
prepare for round 2
-Update datasets for round 2
-Update scripts to reflect round 2
-Rerun model to get new out of sample performance
</commit_message>
<xml_diff>
--- a/Scraping Scripts and Template/Template.xlsx
+++ b/Scraping Scripts and Template/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="46">
   <si>
     <t>Year</t>
   </si>
@@ -162,12 +162,6 @@
   </si>
   <si>
     <t>Team2</t>
-  </si>
-  <si>
-    <t>Washington Capitals/Carolina Hurricanes</t>
-  </si>
-  <si>
-    <t>New York Islanders/Washington Capitals</t>
   </si>
 </sst>
 </file>
@@ -584,14 +578,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="E209" sqref="E209"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
@@ -5017,7 +5011,7 @@
         <v>2019</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>27</v>
@@ -5026,7 +5020,7 @@
         <v>20</v>
       </c>
       <c r="E206" s="5" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F206" s="5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
prepare for round 3
</commit_message>
<xml_diff>
--- a/Scraping Scripts and Template/Template.xlsx
+++ b/Scraping Scripts and Template/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="46">
   <si>
     <t>Year</t>
   </si>
@@ -576,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F208"/>
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="E207" sqref="E207"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5066,6 +5066,46 @@
         <v>24</v>
       </c>
     </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C209" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E209" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F209" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C210" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D210" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E210" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F210" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>